<commit_message>
finished, only needs to complete Readme.md file.
</commit_message>
<xml_diff>
--- a/Input/Kostomlaty/Datasets/Prediction.xlsx
+++ b/Input/Kostomlaty/Datasets/Prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OS\twinbridgegen\Input\Kostomlaty\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6930E016-1CF7-4F38-AF3D-95DA658BA90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7089609C-6FBB-4C46-8F6C-F84168A8BFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C22F6E8-6567-4A6F-97B9-039CA30C3C52}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7C22F6E8-6567-4A6F-97B9-039CA30C3C52}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT ANN" sheetId="1" r:id="rId1"/>
@@ -36,51 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Sample no.</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM12</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM11</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM10</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM09</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM08</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM07</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM06</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM05</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM04</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM03</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM02</t>
-  </si>
-  <si>
-    <t>vlakno-1-avg-strainM01</t>
   </si>
   <si>
     <t>Units</t>
   </si>
   <si>
     <t>[micro-strain]</t>
+  </si>
+  <si>
+    <t>Monitor 1</t>
+  </si>
+  <si>
+    <t>Monitor 2</t>
   </si>
 </sst>
 </file>
@@ -117,13 +87,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD803B5A-4DA0-4531-973B-94D2D52D9CCF}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E4"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,127 +452,37 @@
     <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1.6717573999999998E-4</v>
-      </c>
-      <c r="C3">
-        <v>2.1709521599999997E-4</v>
-      </c>
-      <c r="D3">
-        <v>2.4007607219999998E-4</v>
-      </c>
-      <c r="E3">
-        <v>9.761020689999999E-5</v>
-      </c>
-      <c r="F3">
-        <v>1.4784126E-4</v>
-      </c>
-      <c r="G3">
-        <v>3.020237978E-4</v>
-      </c>
-      <c r="H3">
-        <v>2.129202513E-4</v>
-      </c>
-      <c r="I3">
-        <v>1.2720295600000001E-4</v>
-      </c>
-      <c r="J3">
-        <v>1.725335387E-4</v>
-      </c>
-      <c r="K3">
-        <v>2.3066473389999999E-4</v>
-      </c>
-      <c r="L3">
-        <v>9.3031502999999993E-5</v>
-      </c>
-      <c r="M3">
-        <v>1.9324295889999998E-4</v>
+      <c r="B3" s="2">
+        <v>-1234.0999999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-1168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>